<commit_message>
Docker image standalone successful
</commit_message>
<xml_diff>
--- a/admin/src/main/resources/data/testdata.xlsx
+++ b/admin/src/main/resources/data/testdata.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="test_suite" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -47,7 +48,13 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
+    <t xml:space="preserve">ProductPage</t>
+  </si>
+  <si>
     <t xml:space="preserve">loginTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productPage</t>
   </si>
 </sst>
 </file>
@@ -57,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +94,13 @@
     </font>
     <font>
       <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -143,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,6 +171,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -183,7 +201,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.78"/>
@@ -221,13 +239,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -246,10 +264,26 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -262,4 +296,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>